<commit_message>
Add to the spreadsheet the results of rtb on ZCU102 (FDU, VLD with constants, and VLD with Gaussians) with these options: make build=zup D=CLOCKS,STATS,USE_HASH,USE_OCM,OFFLOAD,VAR_DELAY=_GDT_ RUN_ARGS="-e32Mi -l.60 -c -w1Mi -h.90 -z.99" Note that FDU runs, but VLD hangs on second GDT init.
</commit_message>
<xml_diff>
--- a/misc/results/zup/ZCU102_ADV_vs_SideWinder_Master.xlsx
+++ b/misc/results/zup/ZCU102_ADV_vs_SideWinder_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macaraeg1\Projects\comp\repositories\lime-apps\misc\results\zup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF43073A-2C2F-43D7-8AA3-EC7AA46A4224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16F0245-ED18-458D-B617-C9591C228C68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50" yWindow="2330" windowWidth="29930" windowHeight="15460" tabRatio="633" activeTab="4" xr2:uid="{882556CE-AD92-400A-846D-D6BC51444929}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="633" activeTab="5" xr2:uid="{882556CE-AD92-400A-846D-D6BC51444929}"/>
   </bookViews>
   <sheets>
     <sheet name="zup - image (stock2.txt)" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2583" uniqueCount="877">
   <si>
     <t># make D=CLOCKS,STATS RUN_ARGS="-d&lt;int&gt; -v15 -w24000 -h16000 pat pat"</t>
   </si>
@@ -2595,6 +2595,96 @@
   </si>
   <si>
     <t>CPU 72 1809227 4608 115790528 0</t>
+  </si>
+  <si>
+    <t>aarch64-none-elf-g++ -std=c++11  -O3 -Wall -MMD -DSTATS -DCLOCKS -DUSE_HASH -DZYNQ=_ZU_ -DXILTIME -DUSE_MARGS -DMARGS='"-e32Mi -l.60 -c -w1Mi -h.90 -z.99"' -I../src -Ic:/users/macaraeg1/projects/comp/repositories/lime_master_187.5MHz/shared -Ic:/users/macaraeg1/projects/comp/repositories/lime_master_187.5MHz/shared/standalone -Ic:/users/macaraeg1/projects/comp/repositories/lime_master_187.5MHz/standalone/sdk/standalone_bsp_a53/psu_cortexa53_0/include  -c -o rtb.o ../src/rtb.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> make build=zup D=CLOCKS,STATS,USE_HASH,USE_OCM,OFFLOAD RUN_ARGS="-e32Mi -l.60 -c -w1Mi -h.90 -z.99"</t>
+  </si>
+  <si>
+    <t>aarch64-none-elf-g++ -std=c++11  -O3 -Wall -MMD -DCLOCKS -DSTATS -DUSE_HASH -DUSE_OCM -DOFFLOAD -DUSE_HASH -DZYNQ=_ZU_ -DXILTIME -DUSE_MARGS -DMARGS='"-e32Mi -l.60 -c -w1Mi -h.90 -z.99"' -DUSE_SP -DUSE_OCM -I../src -Ic:/users/macaraeg1/projects/comp/repositories/lime_master_187.5MHz/shared -Ic:/users/macaraeg1/projects/comp/repositories/lime_master_187.5MHz/shared/standalone -Ic:/users/macaraeg1/projects/comp/repositories/lime_master_187.5MHz/standalone/sdk/standalone_bsp_a53/psu_cortexa53_0/include  -c -o rtb.o ../src/rtb.cpp</t>
+  </si>
+  <si>
+    <t>Startup time: 0.721174 sec</t>
+  </si>
+  <si>
+    <t>Insert  rate: 6352573.126293 ops/sec</t>
+  </si>
+  <si>
+    <t>Run     time: 3.737612 sec</t>
+  </si>
+  <si>
+    <t>Oper.   time: 0.567883 sec</t>
+  </si>
+  <si>
+    <t>Insert  time: 3.169729 sec</t>
+  </si>
+  <si>
+    <t>Stats   time: 0.011326 sec</t>
+  </si>
+  <si>
+    <t>Lookup  rate: 30080509.605687 ops/sec</t>
+  </si>
+  <si>
+    <t>Run     time: 0.037343 sec</t>
+  </si>
+  <si>
+    <t>Oper.   time: 0.002484 sec</t>
+  </si>
+  <si>
+    <t>Lookup  time: 0.034859 sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Fill  time: 0.030896 sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cache time: 0.003909 sec</t>
+  </si>
+  <si>
+    <t>CPU 11 65585 704 4197568 0</t>
+  </si>
+  <si>
+    <t>make build=zup D=CLOCKS,STATS,USE_HASH,USE_OCM,OFFLOAD,VAR_DELAY=_GDT_ RUN_ARGS="-e32Mi -l.60 -c -w1Mi -h.90 -z.99"</t>
+  </si>
+  <si>
+    <t>aarch64-none-elf-g++ -std=c++11  -O3 -Wall -MMD -DCLOCKS -DSTATS -DUSE_HASH -DUSE_OCM -DOFFLOAD -DVAR_DELAY=_GDT_ -DUSE_HASH -DZYNQ=_ZU_ -DXILTIME -DUSE_MARGS -DMARGS='"-e32Mi -l.60 -c -w1Mi -h.90 -z.99"' -DUSE_SP -DUSE_OCM -I../src -Ic:/users/macaraeg1/projects/comp/repositories/lime_axi_delayv/shared -Ic:/users/macaraeg1/projects/comp/repositories/lime_axi_delayv/shared/standalone -Ic:/users/macaraeg1/projects/comp/repositories/lime_axi_delayv/standalone/sdk/standalone_bsp_a53/psu_cortexa53_0/include  -c -o rtb.o ../src/rtb.cpp</t>
+  </si>
+  <si>
+    <t>Startup time: 0.738153 sec</t>
+  </si>
+  <si>
+    <t>Insert  rate: 6350996.227181 ops/sec</t>
+  </si>
+  <si>
+    <t>Run     time: 3.738403 sec</t>
+  </si>
+  <si>
+    <t>Oper.   time: 0.567887 sec</t>
+  </si>
+  <si>
+    <t>Insert  time: 3.170516 sec</t>
+  </si>
+  <si>
+    <t>table addr: 0x1000255600</t>
+  </si>
+  <si>
+    <t>heap start:0x1000255080 top:0x1020259000 end:0x10ff255080</t>
+  </si>
+  <si>
+    <t>Insert  rate: 6285505.157571 ops/sec</t>
+  </si>
+  <si>
+    <t>Run     time: 3.771458 sec</t>
+  </si>
+  <si>
+    <t>Oper.   time: 0.567907 sec</t>
+  </si>
+  <si>
+    <t>Insert  time: 3.203551 sec</t>
+  </si>
+  <si>
+    <t>Run 2020-1016</t>
   </si>
 </sst>
 </file>
@@ -2943,7 +3033,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3132,10 +3222,22 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3150,19 +3252,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -21819,17 +21912,17 @@
       <c r="D1" s="33" t="s">
         <v>673</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="74" t="s">
         <v>672</v>
       </c>
-      <c r="F1" s="71"/>
+      <c r="F1" s="75"/>
       <c r="G1" s="33" t="s">
         <v>674</v>
       </c>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="74" t="s">
         <v>672</v>
       </c>
-      <c r="I1" s="71"/>
+      <c r="I1" s="75"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E2" s="44"/>
@@ -23318,8 +23411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620B9BCF-8325-4009-BC05-5CB17AC6287D}">
   <dimension ref="A1:K218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E90" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101:K108"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23952,7 +24045,7 @@
       <c r="C30" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D30" s="74"/>
+      <c r="D30" s="69"/>
       <c r="E30" s="6" t="s">
         <v>175</v>
       </c>
@@ -23962,11 +24055,13 @@
       <c r="A31" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="16"/>
+      <c r="B31" s="16" t="s">
+        <v>847</v>
+      </c>
       <c r="C31" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="D31" s="75"/>
+      <c r="D31" s="70"/>
       <c r="E31" s="7" t="s">
         <v>177</v>
       </c>
@@ -23982,7 +24077,7 @@
       <c r="C32" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="75"/>
+      <c r="D32" s="70"/>
       <c r="E32" s="7" t="s">
         <v>85</v>
       </c>
@@ -23998,7 +24093,7 @@
       <c r="C33" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="75"/>
+      <c r="D33" s="70"/>
       <c r="E33" s="7" t="s">
         <v>86</v>
       </c>
@@ -24014,7 +24109,7 @@
       <c r="C34" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="75"/>
+      <c r="D34" s="70"/>
       <c r="E34" s="7" t="s">
         <v>87</v>
       </c>
@@ -24030,7 +24125,7 @@
       <c r="C35" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="75"/>
+      <c r="D35" s="70"/>
       <c r="E35" s="7" t="s">
         <v>88</v>
       </c>
@@ -24046,7 +24141,7 @@
       <c r="C36" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="75"/>
+      <c r="D36" s="70"/>
       <c r="E36" s="7" t="s">
         <v>89</v>
       </c>
@@ -24057,7 +24152,7 @@
         <v>112</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="75"/>
+      <c r="D37" s="70"/>
       <c r="F37" s="47"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -24070,7 +24165,7 @@
       <c r="C38" s="12" t="s">
         <v>584</v>
       </c>
-      <c r="D38" s="75">
+      <c r="D38" s="70">
         <f>(0.177608-0.170592)/0.170592</f>
         <v>4.1127368223597791E-2</v>
       </c>
@@ -24093,7 +24188,7 @@
       <c r="C39" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="75"/>
+      <c r="D39" s="70"/>
       <c r="E39" s="7" t="s">
         <v>6</v>
       </c>
@@ -24109,7 +24204,7 @@
       <c r="C40" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="75"/>
+      <c r="D40" s="70"/>
       <c r="E40" s="7" t="s">
         <v>7</v>
       </c>
@@ -24125,7 +24220,7 @@
       <c r="C41" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="75"/>
+      <c r="D41" s="70"/>
       <c r="E41" s="7" t="s">
         <v>54</v>
       </c>
@@ -24141,7 +24236,7 @@
       <c r="C42" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="75"/>
+      <c r="D42" s="70"/>
       <c r="E42" s="7" t="s">
         <v>9</v>
       </c>
@@ -24157,7 +24252,7 @@
       <c r="C43" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="75"/>
+      <c r="D43" s="70"/>
       <c r="E43" s="7" t="s">
         <v>55</v>
       </c>
@@ -24173,7 +24268,7 @@
       <c r="C44" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="75"/>
+      <c r="D44" s="70"/>
       <c r="E44" s="7" t="s">
         <v>56</v>
       </c>
@@ -24189,7 +24284,7 @@
       <c r="C45" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="75"/>
+      <c r="D45" s="70"/>
       <c r="E45" s="7" t="s">
         <v>57</v>
       </c>
@@ -24205,7 +24300,7 @@
       <c r="C46" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D46" s="75"/>
+      <c r="D46" s="70"/>
       <c r="E46" s="7" t="s">
         <v>91</v>
       </c>
@@ -24221,7 +24316,7 @@
       <c r="C47" s="12" t="s">
         <v>585</v>
       </c>
-      <c r="D47" s="75">
+      <c r="D47" s="70">
         <f>(4419842.727851-4411063.13737)/4411063.13737</f>
         <v>1.9903570199710768E-3</v>
       </c>
@@ -24254,7 +24349,7 @@
       <c r="C48" s="12" t="s">
         <v>586</v>
       </c>
-      <c r="D48" s="75">
+      <c r="D48" s="70">
         <f>(5.059133-5.06814)/5.06814</f>
         <v>-1.777180583014586E-3</v>
       </c>
@@ -24287,7 +24382,7 @@
       <c r="C49" s="12" t="s">
         <v>587</v>
       </c>
-      <c r="D49" s="75">
+      <c r="D49" s="70">
         <f>(0.481783-0.481679)/0.481679</f>
         <v>2.1591142648941095E-4</v>
       </c>
@@ -24320,7 +24415,7 @@
       <c r="C50" s="12" t="s">
         <v>588</v>
       </c>
-      <c r="D50" s="75">
+      <c r="D50" s="70">
         <f>(4.57735-4.586461)/4.586461</f>
         <v>-1.9864989585651922E-3</v>
       </c>
@@ -24348,7 +24443,7 @@
         <v>119</v>
       </c>
       <c r="C51" s="12"/>
-      <c r="D51" s="75"/>
+      <c r="D51" s="70"/>
       <c r="F51" s="47"/>
       <c r="H51" s="7" t="s">
         <v>805</v>
@@ -24367,7 +24462,7 @@
         <v>120</v>
       </c>
       <c r="C52" s="12"/>
-      <c r="D52" s="75"/>
+      <c r="D52" s="70"/>
       <c r="F52" s="47"/>
       <c r="H52" s="7" t="s">
         <v>802</v>
@@ -24386,7 +24481,7 @@
         <v>121</v>
       </c>
       <c r="C53" s="12"/>
-      <c r="D53" s="75"/>
+      <c r="D53" s="70"/>
       <c r="F53" s="47"/>
       <c r="H53" s="7" t="s">
         <v>791</v>
@@ -24405,7 +24500,7 @@
         <v>122</v>
       </c>
       <c r="C54" s="12"/>
-      <c r="D54" s="75"/>
+      <c r="D54" s="70"/>
       <c r="F54" s="47"/>
       <c r="H54" s="8" t="s">
         <v>806</v>
@@ -24424,7 +24519,7 @@
         <v>123</v>
       </c>
       <c r="C55" s="12"/>
-      <c r="D55" s="76"/>
+      <c r="D55" s="71"/>
       <c r="F55" s="26"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
@@ -24437,7 +24532,7 @@
       <c r="C56" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D56" s="75"/>
+      <c r="D56" s="70"/>
       <c r="E56" s="7" t="s">
         <v>96</v>
       </c>
@@ -24453,7 +24548,7 @@
       <c r="C57" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="75"/>
+      <c r="D57" s="70"/>
       <c r="E57" s="7" t="s">
         <v>97</v>
       </c>
@@ -24470,7 +24565,7 @@
       <c r="C58" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D58" s="75"/>
+      <c r="D58" s="70"/>
       <c r="E58" s="7" t="s">
         <v>98</v>
       </c>
@@ -24486,7 +24581,7 @@
       <c r="C59" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D59" s="75"/>
+      <c r="D59" s="70"/>
       <c r="E59" s="7" t="s">
         <v>99</v>
       </c>
@@ -24502,7 +24597,7 @@
       <c r="C60" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D60" s="75"/>
+      <c r="D60" s="70"/>
       <c r="E60" s="7" t="s">
         <v>178</v>
       </c>
@@ -24518,7 +24613,7 @@
       <c r="C61" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="D61" s="75"/>
+      <c r="D61" s="70"/>
       <c r="E61" s="7" t="s">
         <v>179</v>
       </c>
@@ -24534,7 +24629,7 @@
       <c r="C62" s="12" t="s">
         <v>589</v>
       </c>
-      <c r="D62" s="75">
+      <c r="D62" s="70">
         <f>(20.164347-19.036023)/19.036023</f>
         <v>5.9273095015697302E-2</v>
       </c>
@@ -24556,7 +24651,7 @@
       <c r="C63" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="75"/>
+      <c r="D63" s="70"/>
       <c r="E63" s="7" t="s">
         <v>6</v>
       </c>
@@ -24572,7 +24667,7 @@
       <c r="C64" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="75"/>
+      <c r="D64" s="70"/>
       <c r="E64" s="7" t="s">
         <v>7</v>
       </c>
@@ -24588,7 +24683,7 @@
       <c r="C65" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D65" s="75"/>
+      <c r="D65" s="70"/>
       <c r="E65" s="7" t="s">
         <v>54</v>
       </c>
@@ -24604,7 +24699,7 @@
       <c r="C66" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="75"/>
+      <c r="D66" s="70"/>
       <c r="E66" s="7" t="s">
         <v>9</v>
       </c>
@@ -24620,7 +24715,7 @@
       <c r="C67" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D67" s="75"/>
+      <c r="D67" s="70"/>
       <c r="E67" s="7" t="s">
         <v>55</v>
       </c>
@@ -24636,7 +24731,7 @@
       <c r="C68" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D68" s="75"/>
+      <c r="D68" s="70"/>
       <c r="E68" s="7" t="s">
         <v>56</v>
       </c>
@@ -24652,7 +24747,7 @@
       <c r="C69" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D69" s="75"/>
+      <c r="D69" s="70"/>
       <c r="E69" s="7" t="s">
         <v>57</v>
       </c>
@@ -24668,7 +24763,7 @@
       <c r="C70" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D70" s="75"/>
+      <c r="D70" s="70"/>
       <c r="E70" s="7" t="s">
         <v>103</v>
       </c>
@@ -24684,7 +24779,7 @@
       <c r="C71" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D71" s="75"/>
+      <c r="D71" s="70"/>
       <c r="E71" s="7" t="s">
         <v>104</v>
       </c>
@@ -24700,7 +24795,7 @@
       <c r="C72" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D72" s="75"/>
+      <c r="D72" s="70"/>
       <c r="E72" s="7" t="s">
         <v>105</v>
       </c>
@@ -24716,7 +24811,7 @@
       <c r="C73" s="12" t="s">
         <v>590</v>
       </c>
-      <c r="D73" s="76">
+      <c r="D73" s="71">
         <f>(5424983.706168-5409510.659765)/5409510.659765</f>
         <v>2.8603412353145042E-3</v>
       </c>
@@ -24738,7 +24833,7 @@
       <c r="C74" s="12" t="s">
         <v>591</v>
       </c>
-      <c r="D74" s="76">
+      <c r="D74" s="71">
         <f>(0.195667-0.19622)/0.19622</f>
         <v>-2.8182652125165525E-3</v>
       </c>
@@ -24760,7 +24855,7 @@
       <c r="C75" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="D75" s="76">
+      <c r="D75" s="71">
         <f>(0.002381-0.002381)/0.002381</f>
         <v>0</v>
       </c>
@@ -24782,7 +24877,7 @@
       <c r="C76" s="12" t="s">
         <v>592</v>
       </c>
-      <c r="D76" s="76">
+      <c r="D76" s="71">
         <f>(0.193286-0.193839)/0.193839</f>
         <v>-2.8528830627479397E-3</v>
       </c>
@@ -24800,7 +24895,7 @@
         <v>135</v>
       </c>
       <c r="C77" s="12"/>
-      <c r="D77" s="75"/>
+      <c r="D77" s="70"/>
       <c r="F77" s="47"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
@@ -24808,7 +24903,7 @@
         <v>120</v>
       </c>
       <c r="C78" s="12"/>
-      <c r="D78" s="75"/>
+      <c r="D78" s="70"/>
       <c r="F78" s="47"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -24817,7 +24912,7 @@
       </c>
       <c r="B79" s="16"/>
       <c r="C79" s="12"/>
-      <c r="D79" s="75"/>
+      <c r="D79" s="70"/>
       <c r="E79" s="7"/>
       <c r="F79" s="47"/>
     </row>
@@ -24831,7 +24926,7 @@
       <c r="C80" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D80" s="75"/>
+      <c r="D80" s="70"/>
       <c r="E80" s="7" t="s">
         <v>16</v>
       </c>
@@ -24847,7 +24942,7 @@
       <c r="C81" s="12" t="s">
         <v>593</v>
       </c>
-      <c r="D81" s="75"/>
+      <c r="D81" s="70"/>
       <c r="E81" s="7" t="s">
         <v>768</v>
       </c>
@@ -24859,7 +24954,7 @@
       </c>
       <c r="B82" s="17"/>
       <c r="C82" s="13"/>
-      <c r="D82" s="77"/>
+      <c r="D82" s="72"/>
       <c r="E82" s="8"/>
       <c r="F82" s="48"/>
     </row>
@@ -24875,14 +24970,14 @@
       <c r="A84" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="B84" s="78" t="s">
+      <c r="B84" s="73" t="s">
         <v>814</v>
       </c>
-      <c r="C84" s="78" t="s">
+      <c r="C84" s="73" t="s">
         <v>814</v>
       </c>
       <c r="D84" s="46"/>
-      <c r="E84" s="78" t="s">
+      <c r="E84" s="73" t="s">
         <v>814</v>
       </c>
       <c r="F84" s="46"/>
@@ -25119,14 +25214,14 @@
       <c r="C101" s="7" t="s">
         <v>828</v>
       </c>
-      <c r="D101" s="75">
+      <c r="D101" s="70">
         <f>(4411753.022732-4410573.007165)/4410573.007165</f>
         <v>2.6754246332235797E-4</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>838</v>
       </c>
-      <c r="F101" s="75">
+      <c r="F101" s="70">
         <f>(4345655.991761-4410573.007165)/4410573.007165</f>
         <v>-1.471849922868115E-2</v>
       </c>
@@ -25151,14 +25246,14 @@
       <c r="C102" s="7" t="s">
         <v>829</v>
       </c>
-      <c r="D102" s="75">
+      <c r="D102" s="70">
         <f>(5.067529-5.068654)/5.068654</f>
         <v>-2.2195241576955985E-4</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>839</v>
       </c>
-      <c r="F102" s="75">
+      <c r="F102" s="70">
         <f>(5.137299-5.068654)/5.068654</f>
         <v>1.3543043182667266E-2</v>
       </c>
@@ -25183,14 +25278,14 @@
       <c r="C103" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="D103" s="75">
+      <c r="D103" s="70">
         <f>(0.481785-0.481683)/0.481683</f>
         <v>2.1175752517744347E-4</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>840</v>
       </c>
-      <c r="F103" s="75">
+      <c r="F103" s="70">
         <f>(0.481806-0.481683)/0.481683</f>
         <v>2.5535466271394205E-4</v>
       </c>
@@ -25215,14 +25310,14 @@
       <c r="C104" s="7" t="s">
         <v>831</v>
       </c>
-      <c r="D104" s="75">
+      <c r="D104" s="70">
         <f>(4.585744-4.586971)/4.586971</f>
         <v>-2.6749678600542474E-4</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>841</v>
       </c>
-      <c r="F104" s="75">
+      <c r="F104" s="70">
         <f>(4.655493-4.586971)/4.586971</f>
         <v>1.4938398346098057E-2</v>
       </c>
@@ -25379,14 +25474,14 @@
       <c r="C111" s="7" t="s">
         <v>832</v>
       </c>
-      <c r="D111" s="75">
+      <c r="D111" s="70">
         <f>(20.238777-19.03653)/19.03653</f>
         <v>6.315473460762018E-2</v>
       </c>
       <c r="E111" s="7" t="s">
         <v>842</v>
       </c>
-      <c r="F111" s="75">
+      <c r="F111" s="70">
         <f>(20.242415-19.03653)/19.03653</f>
         <v>6.3345840864905634E-2</v>
       </c>
@@ -25539,14 +25634,14 @@
       <c r="C122" s="7" t="s">
         <v>833</v>
       </c>
-      <c r="D122" s="76">
+      <c r="D122" s="71">
         <f>(5412609.18507-5412221.140987)/5412221.140987</f>
         <v>7.1697750866193117E-5</v>
       </c>
       <c r="E122" s="7" t="s">
         <v>843</v>
       </c>
-      <c r="F122" s="76">
+      <c r="F122" s="71">
         <f>(5355981.808256-5412221.140987)/5412221.140987</f>
         <v>-1.0391174208514336E-2</v>
       </c>
@@ -25559,14 +25654,14 @@
       <c r="C123" s="7" t="s">
         <v>834</v>
       </c>
-      <c r="D123" s="76">
+      <c r="D123" s="71">
         <f>(0.196109-0.196121)/0.196121</f>
         <v>-6.1186716363797078E-5</v>
       </c>
       <c r="E123" s="7" t="s">
         <v>844</v>
       </c>
-      <c r="F123" s="76">
+      <c r="F123" s="71">
         <f>(0.198156-0.196121)/0.196121</f>
         <v>1.0376247316707589E-2</v>
       </c>
@@ -25579,14 +25674,14 @@
       <c r="C124" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="D124" s="76">
+      <c r="D124" s="71">
         <f>(0.002381-0.002378)/0.002378</f>
         <v>1.2615643397813139E-3</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>813</v>
       </c>
-      <c r="F124" s="76">
+      <c r="F124" s="71">
         <f>(0.00238-0.002378)/0.002378</f>
         <v>8.410428931876642E-4</v>
       </c>
@@ -25599,14 +25694,14 @@
       <c r="C125" s="7" t="s">
         <v>835</v>
       </c>
-      <c r="D125" s="76">
+      <c r="D125" s="71">
         <f>(0.193728-0.193742)/0.193742</f>
         <v>-7.2261048198048151E-5</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>845</v>
       </c>
-      <c r="F125" s="76">
+      <c r="F125" s="71">
         <f>(0.195777-0.193742)/0.193742</f>
         <v>1.0503659505940937E-2</v>
       </c>
@@ -26425,10 +26520,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414E3830-8474-43B5-80DD-A953F1321F04}">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K150"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27657,72 +27752,725 @@
       <c r="E85" s="8"/>
       <c r="F85" s="48"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D86" s="49"/>
       <c r="F86" s="49"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C87" s="3" t="s">
+    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B87" s="78" t="s">
+        <v>876</v>
+      </c>
+      <c r="C87" s="78" t="s">
+        <v>876</v>
+      </c>
+      <c r="D87" s="78"/>
+      <c r="E87" s="78" t="s">
+        <v>876</v>
+      </c>
+      <c r="F87" s="79"/>
+    </row>
+    <row r="88" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B88" s="6" t="s">
+        <v>848</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>863</v>
+      </c>
+      <c r="D88" s="46"/>
+      <c r="E88" s="6" t="s">
+        <v>863</v>
+      </c>
+      <c r="F88" s="46"/>
+    </row>
+    <row r="89" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="B89" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="D89" s="47"/>
+      <c r="E89" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="F89" s="47"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B90" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D90" s="47"/>
+      <c r="E90" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F90" s="47"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B91" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D91" s="26"/>
+      <c r="E91" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F91" s="26"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B92" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D92" s="26"/>
+      <c r="E92" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F92" s="26"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B93" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D93" s="26"/>
+      <c r="E93" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F93" s="26"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B94" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D94" s="26"/>
+      <c r="E94" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F94" s="26"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B95" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D95" s="47"/>
+      <c r="E95" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F95" s="47"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B96" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>865</v>
+      </c>
+      <c r="D96" s="26"/>
+      <c r="E96" s="7" t="s">
+        <v>865</v>
+      </c>
+      <c r="F96" s="26"/>
+      <c r="G96" s="5"/>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B97" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="47"/>
+      <c r="E97" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F97" s="47"/>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B98" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="47"/>
+      <c r="E98" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F98" s="47"/>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B99" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D99" s="47"/>
+      <c r="E99" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F99" s="47"/>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B100" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" s="47"/>
+      <c r="E100" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="47"/>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B101" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D101" s="47"/>
+      <c r="E101" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F101" s="47"/>
+    </row>
+    <row r="102" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B102" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D102" s="47"/>
+      <c r="E102" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F102" s="47"/>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B103" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D103" s="47"/>
+      <c r="E103" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F103" s="47"/>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B104" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D104" s="47"/>
+      <c r="E104" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F104" s="47"/>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B105" s="7" t="s">
+        <v>851</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="D105" s="47">
+        <f>(6350996.227181-6352573.126293)/6352573.126293</f>
+        <v>-2.4822998187512698E-4</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>872</v>
+      </c>
+      <c r="F105" s="47">
+        <f>(6285505.157571-6352573.126293)/6352573.126293</f>
+        <v>-1.0557606719143246E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B106" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>867</v>
+      </c>
+      <c r="D106" s="47">
+        <f>(3.738403-3.737612)/3.737612</f>
+        <v>2.1163245409100415E-4</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>873</v>
+      </c>
+      <c r="F106" s="47">
+        <f>(3.771458-3.737612)/3.737612</f>
+        <v>9.0555145905995716E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B107" s="7" t="s">
+        <v>853</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>868</v>
+      </c>
+      <c r="D107" s="47">
+        <f>(0.567887-0.567883)/0.567883</f>
+        <v>7.0437044250382565E-6</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="F107" s="47">
+        <f>(0.567907-0.567883)/0.567883</f>
+        <v>4.2262226550229541E-5</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B108" s="7" t="s">
+        <v>854</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>869</v>
+      </c>
+      <c r="D108" s="47">
+        <f>(3.170516-3.169729)/3.169729</f>
+        <v>2.4828620995684972E-4</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="F108" s="47">
+        <f>(3.203551-3.169729)/3.169729</f>
+        <v>1.0670312824850403E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B109" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D109" s="47"/>
+      <c r="E109" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F109" s="47"/>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B110" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D110" s="47"/>
+      <c r="E110" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F110" s="47"/>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B111" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D111" s="47"/>
+      <c r="E111" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F111" s="47"/>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B112" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>870</v>
+      </c>
+      <c r="D112" s="47"/>
+      <c r="E112" s="7" t="s">
+        <v>870</v>
+      </c>
+      <c r="F112" s="47"/>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B113" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D113" s="47"/>
+      <c r="E113" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F113" s="47"/>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B114" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D114" s="47"/>
+      <c r="E114" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F114" s="47"/>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B115" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D115" s="47"/>
+      <c r="E115" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F115" s="47"/>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B116" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D116" s="47"/>
+      <c r="E116" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F116" s="47"/>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B117" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D117" s="47"/>
+      <c r="E117" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F117" s="47"/>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B118" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>871</v>
+      </c>
+      <c r="D118" s="47"/>
+      <c r="E118" s="7" t="s">
+        <v>871</v>
+      </c>
+      <c r="F118" s="47"/>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B119" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D119" s="47"/>
+      <c r="E119" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F119" s="47"/>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B120" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="D120" s="47"/>
+      <c r="E120" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="F120" s="47"/>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B121" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" s="47"/>
+      <c r="E121" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F121" s="47"/>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B122" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D122" s="47"/>
+      <c r="E122" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F122" s="47"/>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B123" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D123" s="47"/>
+      <c r="E123" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F123" s="47"/>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B124" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" s="47"/>
+      <c r="E124" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F124" s="47"/>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B125" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D125" s="47"/>
+      <c r="E125" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F125" s="47"/>
+    </row>
+    <row r="126" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B126" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D126" s="47"/>
+      <c r="E126" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F126" s="47"/>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B127" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C127" s="7"/>
+      <c r="D127" s="47"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="47"/>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B128" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C128" s="7"/>
+      <c r="D128" s="47"/>
+      <c r="E128" s="7"/>
+      <c r="F128" s="47"/>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B129" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C129" s="7"/>
+      <c r="D129" s="47"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="47"/>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B130" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C130" s="7"/>
+      <c r="D130" s="47"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="47"/>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B131" s="7" t="s">
+        <v>856</v>
+      </c>
+      <c r="C131" s="7"/>
+      <c r="D131" s="47"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="47"/>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B132" s="7" t="s">
+        <v>857</v>
+      </c>
+      <c r="C132" s="7"/>
+      <c r="D132" s="47"/>
+      <c r="E132" s="7"/>
+      <c r="F132" s="47"/>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B133" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="C133" s="7"/>
+      <c r="D133" s="47"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="47"/>
+    </row>
+    <row r="134" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B134" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="C134" s="7"/>
+      <c r="D134" s="47"/>
+      <c r="E134" s="7"/>
+      <c r="F134" s="47"/>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B135" s="7" t="s">
+        <v>860</v>
+      </c>
+      <c r="C135" s="7"/>
+      <c r="D135" s="47"/>
+      <c r="E135" s="7"/>
+      <c r="F135" s="47"/>
+    </row>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B136" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C136" s="7"/>
+      <c r="D136" s="47"/>
+      <c r="E136" s="7"/>
+      <c r="F136" s="47"/>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B137" s="7" t="s">
+        <v>861</v>
+      </c>
+      <c r="C137" s="7"/>
+      <c r="D137" s="47"/>
+      <c r="E137" s="7"/>
+      <c r="F137" s="47"/>
+    </row>
+    <row r="138" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B138" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C138" s="7"/>
+      <c r="D138" s="47"/>
+      <c r="E138" s="7"/>
+      <c r="F138" s="47"/>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B139" s="7" t="s">
+        <v>862</v>
+      </c>
+      <c r="C139" s="7"/>
+      <c r="D139" s="47"/>
+      <c r="E139" s="7"/>
+      <c r="F139" s="47"/>
+    </row>
+    <row r="140" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B140" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C140" s="8"/>
+      <c r="D140" s="48"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="48"/>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C142" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="D87" s="49"/>
-      <c r="F87" s="49"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C88" s="3" t="s">
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C143" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="D88" s="49"/>
-      <c r="F88" s="49"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C89" s="3" t="s">
+    </row>
+    <row r="144" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C144" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="D89" s="49"/>
-      <c r="F89" s="49"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C90" s="3" t="s">
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C145" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="D90" s="68"/>
-      <c r="F90" s="68"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D91" s="68"/>
-      <c r="F91" s="68"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C92" s="3" t="s">
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C147" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="D92" s="68"/>
-      <c r="F92" s="68"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C93" s="3" t="s">
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C148" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="D93" s="68"/>
-      <c r="F93" s="68"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C94" s="3" t="s">
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C149" s="3" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C95" s="3" t="s">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C150" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="D95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -27808,7 +28556,7 @@
         <v>229</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="68" t="s">
         <v>229</v>
       </c>
       <c r="F4" s="18"/>
@@ -29359,13 +30107,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="72"/>
+      <c r="A1" s="76"/>
       <c r="B1" s="19"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="73"/>
+      <c r="A2" s="77"/>
       <c r="B2" s="20"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -29539,13 +30287,13 @@
       <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="72"/>
+      <c r="A31" s="76"/>
       <c r="B31" s="19"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="73"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="20"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>

</xml_diff>